<commit_message>
Activity name changes for samsung
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>USSD_Code</t>
   </si>
@@ -36,50 +36,51 @@
     <t>Test Case Description</t>
   </si>
   <si>
-    <t>TC_USSD_001</t>
-  </si>
-  <si>
-    <t>Test USSD Codes</t>
-  </si>
-  <si>
-    <t>1,22</t>
-  </si>
-  <si>
-    <t>*121*10#</t>
-  </si>
-  <si>
-    <t>TC_USSD_002</t>
-  </si>
-  <si>
-    <t>*121*12#</t>
-  </si>
-  <si>
-    <t>2,22</t>
-  </si>
-  <si>
     <t>Device_Name</t>
   </si>
   <si>
     <t>device1</t>
   </si>
   <si>
-    <t>device2</t>
-  </si>
-  <si>
     <t>Execution_Control</t>
+  </si>
+  <si>
+    <t>CallHomeforLess</t>
+  </si>
+  <si>
+    <t>*135*30#</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>The call home for less offer is active! Call at only 0.6 fils per sec, with a setup fee of AED 1 per call for calls to India, Bangladesh, Pakistan, Afghanistan (except numbers starting with 009378), Egypt, China, Iran, Nepal, Nigeria &amp; Indonesia.</t>
+  </si>
+  <si>
+    <t>As requested, you've been opted out from the New Call Home For Less promotion.</t>
+  </si>
+  <si>
+    <t>CallHomeforLess - OPT IN</t>
+  </si>
+  <si>
+    <t>CallHomeforLess - OPT OUT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Ericsson Hilda"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -98,12 +99,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,21 +407,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1"/>
     <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="176.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -414,47 +440,56 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>